<commit_message>
Home Page components set
</commit_message>
<xml_diff>
--- a/Server/Data/Leaderboard.xlsx
+++ b/Server/Data/Leaderboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KING/Desktop/GitHub/GolfProject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EF857F-D4AB-8D49-A174-740712C0D8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D2F9C5-71D5-CD45-9CDC-2B618BF0AD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D497CE1A-549D-CB4C-BA89-D7D1C7A1E33B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Rank</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Top 10s</t>
-  </si>
-  <si>
-    <t>Stinkers</t>
   </si>
   <si>
     <t>Team</t>
@@ -438,7 +435,7 @@
   <dimension ref="B2:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,10 +448,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -462,9 +459,7 @@
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>